<commit_message>
re-adding in HIV mortality - TB negative trackers
</commit_message>
<xml_diff>
--- a/KZN_south_africa/param_files/Epi_model_parameters.xlsx
+++ b/KZN_south_africa/param_files/Epi_model_parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chelseagreene/github/epi_model_HIV_TB/KZN_south_africa/param_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5304E42-DEB1-2248-8E3C-5154079681CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{956691A0-8CAD-D24B-BDD6-8447DF6C320B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="20560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14920" yWindow="0" windowWidth="20920" windowHeight="20740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="model_matched_parameters" sheetId="1" r:id="rId1"/>
@@ -2751,10 +2751,10 @@
   <dimension ref="A1:Q224"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="119" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="11" ySplit="1" topLeftCell="L224" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="11" ySplit="1" topLeftCell="L2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K1" sqref="K1"/>
+      <selection pane="bottomRight" activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -12241,8 +12241,7 @@
         <v>608</v>
       </c>
       <c r="L217" s="63">
-        <f>1/3</f>
-        <v>0.33333333333333331</v>
+        <v>0.25</v>
       </c>
       <c r="O217" s="55" t="s">
         <v>613</v>
@@ -12275,8 +12274,8 @@
         <v>609</v>
       </c>
       <c r="L218" s="63">
-        <f>0.5</f>
-        <v>0.5</v>
+        <f>1/3</f>
+        <v>0.33333333333333331</v>
       </c>
       <c r="O218" s="55" t="s">
         <v>613</v>
@@ -12309,8 +12308,8 @@
         <v>610</v>
       </c>
       <c r="L219" s="63">
-        <f>0.5</f>
-        <v>0.5</v>
+        <f>1/3</f>
+        <v>0.33333333333333331</v>
       </c>
       <c r="O219" s="55" t="s">
         <v>613</v>
@@ -12343,8 +12342,8 @@
         <v>611</v>
       </c>
       <c r="L220" s="63">
-        <f>0.5</f>
-        <v>0.5</v>
+        <f>1/3</f>
+        <v>0.33333333333333331</v>
       </c>
       <c r="O220" s="35" t="s">
         <v>612</v>
@@ -12478,7 +12477,7 @@
         <v>359</v>
       </c>
       <c r="L224" s="62">
-        <v>0.21</v>
+        <v>0.4</v>
       </c>
       <c r="O224" s="35" t="s">
         <v>593</v>

</xml_diff>